<commit_message>
Entidades modeladas en tablas diferentes, .gitignore
</commit_message>
<xml_diff>
--- a/data/bga-obra.xlsx
+++ b/data/bga-obra.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MI PC\Desktop\Taller Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MI PC\Desktop\Taller Git\bga-obra\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D045B4-6C7F-4601-9CDE-47D290CBBD7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF049FB-19C3-444F-8D81-2469E598A4DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14674" xr2:uid="{918C65DE-BB1A-4AB7-B24F-4654171D12D4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14674" activeTab="2" xr2:uid="{918C65DE-BB1A-4AB7-B24F-4654171D12D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Obra" sheetId="5" r:id="rId2"/>
+    <sheet name="Referente" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -151,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -159,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A855990E-4016-4B2C-878C-5A52CC413A42}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -643,4 +646,211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C33257-496A-4F39-B342-E34FBCAC5B20}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
+  <cols>
+    <col min="2" max="2" width="43.3828125" customWidth="1"/>
+    <col min="3" max="3" width="17.3046875" customWidth="1"/>
+    <col min="4" max="4" width="14.53515625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="14.3828125" customWidth="1"/>
+    <col min="7" max="7" width="25.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1965</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1997</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1983</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C60AB4-B36D-49B4-A9A5-F74E617BBC21}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
+  <cols>
+    <col min="2" max="2" width="43.3828125" customWidth="1"/>
+    <col min="3" max="3" width="17.3046875" customWidth="1"/>
+    <col min="4" max="4" width="14.3828125" customWidth="1"/>
+    <col min="5" max="5" width="25.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>